<commit_message>
Matriz GUT ordenada de forma DECRESCENTE, dessa forma fica mais facil visualizar a ordem dos items a serem atacados.
</commit_message>
<xml_diff>
--- a/4.Improve/Matriz GUT/Matriz GUT - TRE.xlsx
+++ b/4.Improve/Matriz GUT/Matriz GUT - TRE.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\e047697\Documents\Puc_Lean_2016\Improve\Matriz GUT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Andre\PUCPR POS\Puc_Lean2016\4.Improve\Matriz GUT\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -13,8 +13,10 @@
   </bookViews>
   <sheets>
     <sheet name="Matriz GUT" sheetId="1" r:id="rId1"/>
+    <sheet name="GUT Ordenada" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'GUT Ordenada'!$A$1:$F$10</definedName>
     <definedName name="Gravidade" localSheetId="0">'Matriz GUT'!$B$3</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
@@ -22,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="34">
   <si>
     <t>Modelo GUT</t>
   </si>
@@ -372,7 +374,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -416,15 +418,6 @@
     <xf numFmtId="0" fontId="5" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -438,6 +431,43 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -780,8 +810,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL232"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -799,14 +829,14 @@
   <sheetData>
     <row r="1" spans="1:38" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="24"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="21"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
@@ -841,14 +871,14 @@
     </row>
     <row r="2" spans="1:38" ht="75.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="24"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="21"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
@@ -883,10 +913,10 @@
     </row>
     <row r="3" spans="1:38" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3"/>
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="27"/>
+      <c r="C3" s="24"/>
       <c r="D3" s="4" t="s">
         <v>1</v>
       </c>
@@ -933,24 +963,24 @@
       <c r="AK3" s="8"/>
       <c r="AL3" s="8"/>
     </row>
-    <row r="4" spans="1:38" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:38" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
-      <c r="B4" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="C4" s="20"/>
-      <c r="D4" s="10">
-        <v>3</v>
-      </c>
-      <c r="E4" s="11">
-        <v>3</v>
-      </c>
-      <c r="F4" s="12">
-        <v>1</v>
-      </c>
-      <c r="G4" s="13">
+      <c r="B4" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="31"/>
+      <c r="D4" s="34">
+        <v>5</v>
+      </c>
+      <c r="E4" s="35">
+        <v>5</v>
+      </c>
+      <c r="F4" s="36">
+        <v>5</v>
+      </c>
+      <c r="G4" s="37">
         <f t="shared" ref="G4:G32" si="0">D4+E4+F4</f>
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="H4" s="2"/>
       <c r="I4" s="14" t="s">
@@ -959,44 +989,44 @@
     </row>
     <row r="5" spans="1:38" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
-      <c r="B5" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" s="20"/>
-      <c r="D5" s="10">
+      <c r="B5" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="33"/>
+      <c r="D5" s="34">
+        <v>3</v>
+      </c>
+      <c r="E5" s="35">
         <v>5</v>
       </c>
-      <c r="E5" s="11">
-        <v>5</v>
-      </c>
-      <c r="F5" s="12">
-        <v>1</v>
-      </c>
-      <c r="G5" s="13">
+      <c r="F5" s="36">
+        <v>4</v>
+      </c>
+      <c r="G5" s="37">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H5" s="2"/>
       <c r="I5" s="14" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:38" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:38" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
-      <c r="B6" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="C6" s="20"/>
-      <c r="D6" s="10">
-        <v>3</v>
-      </c>
-      <c r="E6" s="11">
-        <v>5</v>
-      </c>
-      <c r="F6" s="12">
+      <c r="B6" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="33"/>
+      <c r="D6" s="34">
         <v>4</v>
       </c>
-      <c r="G6" s="13">
+      <c r="E6" s="35">
+        <v>4</v>
+      </c>
+      <c r="F6" s="36">
+        <v>4</v>
+      </c>
+      <c r="G6" s="37">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
@@ -1007,22 +1037,22 @@
     </row>
     <row r="7" spans="1:38" ht="28.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
-      <c r="B7" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" s="20"/>
-      <c r="D7" s="10">
+      <c r="B7" s="30" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="31"/>
+      <c r="D7" s="34">
         <v>5</v>
       </c>
-      <c r="E7" s="11">
+      <c r="E7" s="35">
         <v>5</v>
       </c>
-      <c r="F7" s="12">
-        <v>5</v>
-      </c>
-      <c r="G7" s="13">
+      <c r="F7" s="36">
+        <v>1</v>
+      </c>
+      <c r="G7" s="37">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="H7" s="2"/>
       <c r="I7" s="14" t="s">
@@ -1031,90 +1061,90 @@
     </row>
     <row r="8" spans="1:38" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
-      <c r="B8" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="C8" s="20"/>
-      <c r="D8" s="10">
-        <v>2</v>
-      </c>
-      <c r="E8" s="11">
-        <v>2</v>
-      </c>
-      <c r="F8" s="12">
-        <v>2</v>
-      </c>
-      <c r="G8" s="13">
+      <c r="B8" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="33"/>
+      <c r="D8" s="34">
+        <v>4</v>
+      </c>
+      <c r="E8" s="35">
+        <v>4</v>
+      </c>
+      <c r="F8" s="36">
+        <v>3</v>
+      </c>
+      <c r="G8" s="37">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="H8" s="2"/>
       <c r="I8" s="14" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:38" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:38" ht="32.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
-      <c r="B9" s="21" t="s">
+      <c r="B9" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="20"/>
-      <c r="D9" s="10">
+      <c r="C9" s="33"/>
+      <c r="D9" s="34">
         <v>2</v>
       </c>
-      <c r="E9" s="11">
+      <c r="E9" s="35">
         <v>3</v>
       </c>
-      <c r="F9" s="12">
+      <c r="F9" s="36">
         <v>3</v>
       </c>
-      <c r="G9" s="13">
+      <c r="G9" s="37">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="H9" s="2"/>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:38" ht="29.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:38" ht="31.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
-      <c r="B10" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="C10" s="20"/>
-      <c r="D10" s="10">
-        <v>4</v>
-      </c>
-      <c r="E10" s="11">
-        <v>4</v>
-      </c>
-      <c r="F10" s="12">
-        <v>4</v>
-      </c>
-      <c r="G10" s="13">
+      <c r="B10" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="31"/>
+      <c r="D10" s="34">
+        <v>3</v>
+      </c>
+      <c r="E10" s="35">
+        <v>3</v>
+      </c>
+      <c r="F10" s="36">
+        <v>1</v>
+      </c>
+      <c r="G10" s="37">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="H10" s="2"/>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:38" ht="38.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:38" ht="31.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
-      <c r="B11" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="C11" s="20"/>
-      <c r="D11" s="10">
-        <v>4</v>
-      </c>
-      <c r="E11" s="11">
-        <v>4</v>
-      </c>
-      <c r="F11" s="12">
-        <v>3</v>
-      </c>
-      <c r="G11" s="13">
+      <c r="B11" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="31"/>
+      <c r="D11" s="34">
+        <v>2</v>
+      </c>
+      <c r="E11" s="35">
+        <v>2</v>
+      </c>
+      <c r="F11" s="36">
+        <v>2</v>
+      </c>
+      <c r="G11" s="37">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="H11" s="2"/>
       <c r="I11" s="15" t="s">
@@ -1123,20 +1153,20 @@
     </row>
     <row r="12" spans="1:38" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
-      <c r="B12" s="21" t="s">
+      <c r="B12" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="C12" s="20"/>
-      <c r="D12" s="10">
+      <c r="C12" s="33"/>
+      <c r="D12" s="34">
         <v>2</v>
       </c>
-      <c r="E12" s="11">
+      <c r="E12" s="35">
         <v>2</v>
       </c>
-      <c r="F12" s="12">
+      <c r="F12" s="36">
         <v>2</v>
       </c>
-      <c r="G12" s="13">
+      <c r="G12" s="37">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
@@ -1147,8 +1177,8 @@
     </row>
     <row r="13" spans="1:38" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
-      <c r="B13" s="19"/>
-      <c r="C13" s="20"/>
+      <c r="B13" s="25"/>
+      <c r="C13" s="26"/>
       <c r="D13" s="10"/>
       <c r="E13" s="11"/>
       <c r="F13" s="12"/>
@@ -1163,8 +1193,8 @@
     </row>
     <row r="14" spans="1:38" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
-      <c r="B14" s="19"/>
-      <c r="C14" s="20"/>
+      <c r="B14" s="25"/>
+      <c r="C14" s="26"/>
       <c r="D14" s="10"/>
       <c r="E14" s="11"/>
       <c r="F14" s="12"/>
@@ -1179,8 +1209,8 @@
     </row>
     <row r="15" spans="1:38" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
-      <c r="B15" s="19"/>
-      <c r="C15" s="20"/>
+      <c r="B15" s="25"/>
+      <c r="C15" s="26"/>
       <c r="D15" s="10"/>
       <c r="E15" s="11"/>
       <c r="F15" s="12"/>
@@ -1195,8 +1225,8 @@
     </row>
     <row r="16" spans="1:38" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
-      <c r="B16" s="19"/>
-      <c r="C16" s="20"/>
+      <c r="B16" s="25"/>
+      <c r="C16" s="26"/>
       <c r="D16" s="10"/>
       <c r="E16" s="11"/>
       <c r="F16" s="12"/>
@@ -1211,8 +1241,8 @@
     </row>
     <row r="17" spans="1:38" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
-      <c r="B17" s="19"/>
-      <c r="C17" s="20"/>
+      <c r="B17" s="25"/>
+      <c r="C17" s="26"/>
       <c r="D17" s="10"/>
       <c r="E17" s="11"/>
       <c r="F17" s="12"/>
@@ -1225,8 +1255,8 @@
     </row>
     <row r="18" spans="1:38" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
-      <c r="B18" s="19"/>
-      <c r="C18" s="20"/>
+      <c r="B18" s="25"/>
+      <c r="C18" s="26"/>
       <c r="D18" s="10"/>
       <c r="E18" s="11"/>
       <c r="F18" s="12"/>
@@ -1239,8 +1269,8 @@
     </row>
     <row r="19" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
-      <c r="B19" s="19"/>
-      <c r="C19" s="20"/>
+      <c r="B19" s="25"/>
+      <c r="C19" s="26"/>
       <c r="D19" s="10"/>
       <c r="E19" s="11"/>
       <c r="F19" s="12"/>
@@ -1255,8 +1285,8 @@
     </row>
     <row r="20" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
-      <c r="B20" s="19"/>
-      <c r="C20" s="20"/>
+      <c r="B20" s="25"/>
+      <c r="C20" s="26"/>
       <c r="D20" s="10"/>
       <c r="E20" s="11"/>
       <c r="F20" s="12"/>
@@ -1271,8 +1301,8 @@
     </row>
     <row r="21" spans="1:38" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
-      <c r="B21" s="19"/>
-      <c r="C21" s="20"/>
+      <c r="B21" s="25"/>
+      <c r="C21" s="26"/>
       <c r="D21" s="10"/>
       <c r="E21" s="11"/>
       <c r="F21" s="12"/>
@@ -1287,8 +1317,8 @@
     </row>
     <row r="22" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
-      <c r="B22" s="19"/>
-      <c r="C22" s="20"/>
+      <c r="B22" s="25"/>
+      <c r="C22" s="26"/>
       <c r="D22" s="10"/>
       <c r="E22" s="11"/>
       <c r="F22" s="12"/>
@@ -1303,8 +1333,8 @@
     </row>
     <row r="23" spans="1:38" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
-      <c r="B23" s="19"/>
-      <c r="C23" s="20"/>
+      <c r="B23" s="25"/>
+      <c r="C23" s="26"/>
       <c r="D23" s="10"/>
       <c r="E23" s="11"/>
       <c r="F23" s="12"/>
@@ -1319,8 +1349,8 @@
     </row>
     <row r="24" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
-      <c r="B24" s="19"/>
-      <c r="C24" s="20"/>
+      <c r="B24" s="25"/>
+      <c r="C24" s="26"/>
       <c r="D24" s="10"/>
       <c r="E24" s="11"/>
       <c r="F24" s="12"/>
@@ -1335,8 +1365,8 @@
     </row>
     <row r="25" spans="1:38" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
-      <c r="B25" s="19"/>
-      <c r="C25" s="20"/>
+      <c r="B25" s="25"/>
+      <c r="C25" s="26"/>
       <c r="D25" s="10"/>
       <c r="E25" s="11"/>
       <c r="F25" s="12"/>
@@ -1349,8 +1379,8 @@
     </row>
     <row r="26" spans="1:38" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
-      <c r="B26" s="19"/>
-      <c r="C26" s="20"/>
+      <c r="B26" s="25"/>
+      <c r="C26" s="26"/>
       <c r="D26" s="10"/>
       <c r="E26" s="11"/>
       <c r="F26" s="12"/>
@@ -1363,8 +1393,8 @@
     </row>
     <row r="27" spans="1:38" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
-      <c r="B27" s="19"/>
-      <c r="C27" s="20"/>
+      <c r="B27" s="25"/>
+      <c r="C27" s="26"/>
       <c r="D27" s="10"/>
       <c r="E27" s="11"/>
       <c r="F27" s="12"/>
@@ -1377,8 +1407,8 @@
     </row>
     <row r="28" spans="1:38" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
-      <c r="B28" s="19"/>
-      <c r="C28" s="20"/>
+      <c r="B28" s="25"/>
+      <c r="C28" s="26"/>
       <c r="D28" s="10"/>
       <c r="E28" s="11"/>
       <c r="F28" s="12"/>
@@ -1391,8 +1421,8 @@
     </row>
     <row r="29" spans="1:38" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
-      <c r="B29" s="19"/>
-      <c r="C29" s="20"/>
+      <c r="B29" s="25"/>
+      <c r="C29" s="26"/>
       <c r="D29" s="10"/>
       <c r="E29" s="11"/>
       <c r="F29" s="12"/>
@@ -1405,8 +1435,8 @@
     </row>
     <row r="30" spans="1:38" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
-      <c r="B30" s="19"/>
-      <c r="C30" s="20"/>
+      <c r="B30" s="25"/>
+      <c r="C30" s="26"/>
       <c r="D30" s="10"/>
       <c r="E30" s="11"/>
       <c r="F30" s="12"/>
@@ -1419,8 +1449,8 @@
     </row>
     <row r="31" spans="1:38" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
-      <c r="B31" s="19"/>
-      <c r="C31" s="20"/>
+      <c r="B31" s="25"/>
+      <c r="C31" s="26"/>
       <c r="D31" s="10"/>
       <c r="E31" s="11"/>
       <c r="F31" s="12"/>
@@ -1433,8 +1463,8 @@
     </row>
     <row r="32" spans="1:38" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
-      <c r="B32" s="19"/>
-      <c r="C32" s="20"/>
+      <c r="B32" s="25"/>
+      <c r="C32" s="26"/>
       <c r="D32" s="10"/>
       <c r="E32" s="11"/>
       <c r="F32" s="12"/>
@@ -9476,31 +9506,6 @@
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="B1:G1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B25:C25"/>
     <mergeCell ref="B31:C31"/>
     <mergeCell ref="B32:C32"/>
     <mergeCell ref="B26:C26"/>
@@ -9508,8 +9513,246 @@
     <mergeCell ref="B28:C28"/>
     <mergeCell ref="B29:C29"/>
     <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="85.77734375" customWidth="1"/>
+    <col min="2" max="2" width="7.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="29"/>
+      <c r="C1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A2" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="27"/>
+      <c r="C2" s="10">
+        <v>5</v>
+      </c>
+      <c r="D2" s="11">
+        <v>5</v>
+      </c>
+      <c r="E2" s="12">
+        <v>5</v>
+      </c>
+      <c r="F2" s="13">
+        <f>C2+D2+E2</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="28"/>
+      <c r="C3" s="10">
+        <v>3</v>
+      </c>
+      <c r="D3" s="11">
+        <v>5</v>
+      </c>
+      <c r="E3" s="12">
+        <v>4</v>
+      </c>
+      <c r="F3" s="13">
+        <f>C3+D3+E3</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A4" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="28"/>
+      <c r="C4" s="10">
+        <v>4</v>
+      </c>
+      <c r="D4" s="11">
+        <v>4</v>
+      </c>
+      <c r="E4" s="12">
+        <v>4</v>
+      </c>
+      <c r="F4" s="13">
+        <f>C4+D4+E4</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A5" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="27"/>
+      <c r="C5" s="10">
+        <v>5</v>
+      </c>
+      <c r="D5" s="11">
+        <v>5</v>
+      </c>
+      <c r="E5" s="12">
+        <v>1</v>
+      </c>
+      <c r="F5" s="13">
+        <f>C5+D5+E5</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A6" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="28"/>
+      <c r="C6" s="10">
+        <v>4</v>
+      </c>
+      <c r="D6" s="11">
+        <v>4</v>
+      </c>
+      <c r="E6" s="12">
+        <v>3</v>
+      </c>
+      <c r="F6" s="13">
+        <f>C6+D6+E6</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A7" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="28"/>
+      <c r="C7" s="10">
+        <v>2</v>
+      </c>
+      <c r="D7" s="11">
+        <v>3</v>
+      </c>
+      <c r="E7" s="12">
+        <v>3</v>
+      </c>
+      <c r="F7" s="13">
+        <f>C7+D7+E7</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A8" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="27"/>
+      <c r="C8" s="10">
+        <v>3</v>
+      </c>
+      <c r="D8" s="11">
+        <v>3</v>
+      </c>
+      <c r="E8" s="12">
+        <v>1</v>
+      </c>
+      <c r="F8" s="13">
+        <f>C8+D8+E8</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A9" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="27"/>
+      <c r="C9" s="10">
+        <v>2</v>
+      </c>
+      <c r="D9" s="11">
+        <v>2</v>
+      </c>
+      <c r="E9" s="12">
+        <v>2</v>
+      </c>
+      <c r="F9" s="13">
+        <f>C9+D9+E9</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="28"/>
+      <c r="C10" s="10">
+        <v>2</v>
+      </c>
+      <c r="D10" s="11">
+        <v>2</v>
+      </c>
+      <c r="E10" s="12">
+        <v>2</v>
+      </c>
+      <c r="F10" s="13">
+        <f>C10+D10+E10</f>
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:F10">
+    <sortState ref="A2:F10">
+      <sortCondition descending="1" ref="F1:F10"/>
+    </sortState>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
A Matrix GUT está na sessão IMPROVE - "Será necessário priorizar as soluções?" E a Matriz 5W2H está dentro de "Será necessário testar as soluções? Como os testes serão realizados?"
</commit_message>
<xml_diff>
--- a/4.Improve/Matriz GUT/Matriz GUT - TRE.xlsx
+++ b/4.Improve/Matriz GUT/Matriz GUT - TRE.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9000"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9000" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Matriz GUT" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="40">
   <si>
     <t>Modelo GUT</t>
   </si>
@@ -142,6 +142,24 @@
   </si>
   <si>
     <t>Criar um fluxo de aprovação de alteracao nos modelos criados na pasta K</t>
+  </si>
+  <si>
+    <t>Treinamentos sobre o que será inspecionado nos documentos e interessados sejam notificados.</t>
+  </si>
+  <si>
+    <t>Utilização de tecnicas de desenvolvimento agil como ( Kanban e Stand Up meetings ) para alinhar o trabalho.</t>
+  </si>
+  <si>
+    <t>Versionamento de Documentos para evitar duplicidades com criação de uma pasta compartilhada na rede.</t>
+  </si>
+  <si>
+    <t>Criação de um repositório de conhecimento onde alterações nos MODELOS sejam replicadas mais rapidamente e as pessoas sejam notificadas destas mudanças.</t>
+  </si>
+  <si>
+    <t>Padronização de Códigos para inserção de Comentários evitando baixo rastreamento dos retornos dos PADS (por exemplo: para ciencia, para correção,  . ).</t>
+  </si>
+  <si>
+    <t>Criar um fluxo de aprovação de alteracao nos modelos criados na pasta K.</t>
   </si>
 </sst>
 </file>
@@ -418,6 +436,43 @@
     <xf numFmtId="0" fontId="5" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -431,43 +486,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -810,7 +828,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL232"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B4" sqref="B4:C4"/>
     </sheetView>
   </sheetViews>
@@ -829,14 +847,14 @@
   <sheetData>
     <row r="1" spans="1:38" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="21"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="34"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
@@ -871,14 +889,14 @@
     </row>
     <row r="2" spans="1:38" ht="75.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="21"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="34"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
@@ -913,10 +931,10 @@
     </row>
     <row r="3" spans="1:38" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3"/>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="24"/>
+      <c r="C3" s="37"/>
       <c r="D3" s="4" t="s">
         <v>1</v>
       </c>
@@ -965,20 +983,20 @@
     </row>
     <row r="4" spans="1:38" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="31"/>
-      <c r="D4" s="34">
+      <c r="C4" s="29"/>
+      <c r="D4" s="22">
         <v>5</v>
       </c>
-      <c r="E4" s="35">
+      <c r="E4" s="23">
         <v>5</v>
       </c>
-      <c r="F4" s="36">
+      <c r="F4" s="24">
         <v>5</v>
       </c>
-      <c r="G4" s="37">
+      <c r="G4" s="25">
         <f t="shared" ref="G4:G32" si="0">D4+E4+F4</f>
         <v>15</v>
       </c>
@@ -989,20 +1007,20 @@
     </row>
     <row r="5" spans="1:38" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
-      <c r="B5" s="32" t="s">
+      <c r="B5" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="33"/>
-      <c r="D5" s="34">
+      <c r="C5" s="31"/>
+      <c r="D5" s="22">
         <v>3</v>
       </c>
-      <c r="E5" s="35">
+      <c r="E5" s="23">
         <v>5</v>
       </c>
-      <c r="F5" s="36">
+      <c r="F5" s="24">
         <v>4</v>
       </c>
-      <c r="G5" s="37">
+      <c r="G5" s="25">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
@@ -1013,20 +1031,20 @@
     </row>
     <row r="6" spans="1:38" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
-      <c r="B6" s="32" t="s">
+      <c r="B6" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="33"/>
-      <c r="D6" s="34">
+      <c r="C6" s="31"/>
+      <c r="D6" s="22">
         <v>4</v>
       </c>
-      <c r="E6" s="35">
+      <c r="E6" s="23">
         <v>4</v>
       </c>
-      <c r="F6" s="36">
+      <c r="F6" s="24">
         <v>4</v>
       </c>
-      <c r="G6" s="37">
+      <c r="G6" s="25">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
@@ -1037,20 +1055,20 @@
     </row>
     <row r="7" spans="1:38" ht="28.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
-      <c r="B7" s="30" t="s">
+      <c r="B7" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="31"/>
-      <c r="D7" s="34">
+      <c r="C7" s="29"/>
+      <c r="D7" s="22">
         <v>5</v>
       </c>
-      <c r="E7" s="35">
+      <c r="E7" s="23">
         <v>5</v>
       </c>
-      <c r="F7" s="36">
+      <c r="F7" s="24">
         <v>1</v>
       </c>
-      <c r="G7" s="37">
+      <c r="G7" s="25">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
@@ -1061,20 +1079,20 @@
     </row>
     <row r="8" spans="1:38" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
-      <c r="B8" s="32" t="s">
+      <c r="B8" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="33"/>
-      <c r="D8" s="34">
+      <c r="C8" s="31"/>
+      <c r="D8" s="22">
         <v>4</v>
       </c>
-      <c r="E8" s="35">
+      <c r="E8" s="23">
         <v>4</v>
       </c>
-      <c r="F8" s="36">
+      <c r="F8" s="24">
         <v>3</v>
       </c>
-      <c r="G8" s="37">
+      <c r="G8" s="25">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
@@ -1085,20 +1103,20 @@
     </row>
     <row r="9" spans="1:38" ht="32.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
-      <c r="B9" s="32" t="s">
+      <c r="B9" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="33"/>
-      <c r="D9" s="34">
+      <c r="C9" s="31"/>
+      <c r="D9" s="22">
         <v>2</v>
       </c>
-      <c r="E9" s="35">
+      <c r="E9" s="23">
         <v>3</v>
       </c>
-      <c r="F9" s="36">
+      <c r="F9" s="24">
         <v>3</v>
       </c>
-      <c r="G9" s="37">
+      <c r="G9" s="25">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
@@ -1107,20 +1125,20 @@
     </row>
     <row r="10" spans="1:38" ht="31.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
-      <c r="B10" s="30" t="s">
+      <c r="B10" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="31"/>
-      <c r="D10" s="34">
+      <c r="C10" s="29"/>
+      <c r="D10" s="22">
         <v>3</v>
       </c>
-      <c r="E10" s="35">
+      <c r="E10" s="23">
         <v>3</v>
       </c>
-      <c r="F10" s="36">
+      <c r="F10" s="24">
         <v>1</v>
       </c>
-      <c r="G10" s="37">
+      <c r="G10" s="25">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
@@ -1129,20 +1147,20 @@
     </row>
     <row r="11" spans="1:38" ht="31.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
-      <c r="B11" s="30" t="s">
+      <c r="B11" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="31"/>
-      <c r="D11" s="34">
+      <c r="C11" s="29"/>
+      <c r="D11" s="22">
         <v>2</v>
       </c>
-      <c r="E11" s="35">
+      <c r="E11" s="23">
         <v>2</v>
       </c>
-      <c r="F11" s="36">
+      <c r="F11" s="24">
         <v>2</v>
       </c>
-      <c r="G11" s="37">
+      <c r="G11" s="25">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
@@ -1153,20 +1171,20 @@
     </row>
     <row r="12" spans="1:38" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
-      <c r="B12" s="32" t="s">
+      <c r="B12" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="C12" s="33"/>
-      <c r="D12" s="34">
+      <c r="C12" s="31"/>
+      <c r="D12" s="22">
         <v>2</v>
       </c>
-      <c r="E12" s="35">
+      <c r="E12" s="23">
         <v>2</v>
       </c>
-      <c r="F12" s="36">
+      <c r="F12" s="24">
         <v>2</v>
       </c>
-      <c r="G12" s="37">
+      <c r="G12" s="25">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
@@ -1177,8 +1195,8 @@
     </row>
     <row r="13" spans="1:38" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
-      <c r="B13" s="25"/>
-      <c r="C13" s="26"/>
+      <c r="B13" s="26"/>
+      <c r="C13" s="27"/>
       <c r="D13" s="10"/>
       <c r="E13" s="11"/>
       <c r="F13" s="12"/>
@@ -1193,8 +1211,8 @@
     </row>
     <row r="14" spans="1:38" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
-      <c r="B14" s="25"/>
-      <c r="C14" s="26"/>
+      <c r="B14" s="26"/>
+      <c r="C14" s="27"/>
       <c r="D14" s="10"/>
       <c r="E14" s="11"/>
       <c r="F14" s="12"/>
@@ -1209,8 +1227,8 @@
     </row>
     <row r="15" spans="1:38" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
-      <c r="B15" s="25"/>
-      <c r="C15" s="26"/>
+      <c r="B15" s="26"/>
+      <c r="C15" s="27"/>
       <c r="D15" s="10"/>
       <c r="E15" s="11"/>
       <c r="F15" s="12"/>
@@ -1225,8 +1243,8 @@
     </row>
     <row r="16" spans="1:38" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
-      <c r="B16" s="25"/>
-      <c r="C16" s="26"/>
+      <c r="B16" s="26"/>
+      <c r="C16" s="27"/>
       <c r="D16" s="10"/>
       <c r="E16" s="11"/>
       <c r="F16" s="12"/>
@@ -1241,8 +1259,8 @@
     </row>
     <row r="17" spans="1:38" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
-      <c r="B17" s="25"/>
-      <c r="C17" s="26"/>
+      <c r="B17" s="26"/>
+      <c r="C17" s="27"/>
       <c r="D17" s="10"/>
       <c r="E17" s="11"/>
       <c r="F17" s="12"/>
@@ -1255,8 +1273,8 @@
     </row>
     <row r="18" spans="1:38" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
-      <c r="B18" s="25"/>
-      <c r="C18" s="26"/>
+      <c r="B18" s="26"/>
+      <c r="C18" s="27"/>
       <c r="D18" s="10"/>
       <c r="E18" s="11"/>
       <c r="F18" s="12"/>
@@ -1269,8 +1287,8 @@
     </row>
     <row r="19" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
-      <c r="B19" s="25"/>
-      <c r="C19" s="26"/>
+      <c r="B19" s="26"/>
+      <c r="C19" s="27"/>
       <c r="D19" s="10"/>
       <c r="E19" s="11"/>
       <c r="F19" s="12"/>
@@ -1285,8 +1303,8 @@
     </row>
     <row r="20" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
-      <c r="B20" s="25"/>
-      <c r="C20" s="26"/>
+      <c r="B20" s="26"/>
+      <c r="C20" s="27"/>
       <c r="D20" s="10"/>
       <c r="E20" s="11"/>
       <c r="F20" s="12"/>
@@ -1301,8 +1319,8 @@
     </row>
     <row r="21" spans="1:38" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
-      <c r="B21" s="25"/>
-      <c r="C21" s="26"/>
+      <c r="B21" s="26"/>
+      <c r="C21" s="27"/>
       <c r="D21" s="10"/>
       <c r="E21" s="11"/>
       <c r="F21" s="12"/>
@@ -1317,8 +1335,8 @@
     </row>
     <row r="22" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
-      <c r="B22" s="25"/>
-      <c r="C22" s="26"/>
+      <c r="B22" s="26"/>
+      <c r="C22" s="27"/>
       <c r="D22" s="10"/>
       <c r="E22" s="11"/>
       <c r="F22" s="12"/>
@@ -1333,8 +1351,8 @@
     </row>
     <row r="23" spans="1:38" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
-      <c r="B23" s="25"/>
-      <c r="C23" s="26"/>
+      <c r="B23" s="26"/>
+      <c r="C23" s="27"/>
       <c r="D23" s="10"/>
       <c r="E23" s="11"/>
       <c r="F23" s="12"/>
@@ -1349,8 +1367,8 @@
     </row>
     <row r="24" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
-      <c r="B24" s="25"/>
-      <c r="C24" s="26"/>
+      <c r="B24" s="26"/>
+      <c r="C24" s="27"/>
       <c r="D24" s="10"/>
       <c r="E24" s="11"/>
       <c r="F24" s="12"/>
@@ -1365,8 +1383,8 @@
     </row>
     <row r="25" spans="1:38" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
-      <c r="B25" s="25"/>
-      <c r="C25" s="26"/>
+      <c r="B25" s="26"/>
+      <c r="C25" s="27"/>
       <c r="D25" s="10"/>
       <c r="E25" s="11"/>
       <c r="F25" s="12"/>
@@ -1379,8 +1397,8 @@
     </row>
     <row r="26" spans="1:38" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
-      <c r="B26" s="25"/>
-      <c r="C26" s="26"/>
+      <c r="B26" s="26"/>
+      <c r="C26" s="27"/>
       <c r="D26" s="10"/>
       <c r="E26" s="11"/>
       <c r="F26" s="12"/>
@@ -1393,8 +1411,8 @@
     </row>
     <row r="27" spans="1:38" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
-      <c r="B27" s="25"/>
-      <c r="C27" s="26"/>
+      <c r="B27" s="26"/>
+      <c r="C27" s="27"/>
       <c r="D27" s="10"/>
       <c r="E27" s="11"/>
       <c r="F27" s="12"/>
@@ -1407,8 +1425,8 @@
     </row>
     <row r="28" spans="1:38" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
-      <c r="B28" s="25"/>
-      <c r="C28" s="26"/>
+      <c r="B28" s="26"/>
+      <c r="C28" s="27"/>
       <c r="D28" s="10"/>
       <c r="E28" s="11"/>
       <c r="F28" s="12"/>
@@ -1421,8 +1439,8 @@
     </row>
     <row r="29" spans="1:38" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
-      <c r="B29" s="25"/>
-      <c r="C29" s="26"/>
+      <c r="B29" s="26"/>
+      <c r="C29" s="27"/>
       <c r="D29" s="10"/>
       <c r="E29" s="11"/>
       <c r="F29" s="12"/>
@@ -1435,8 +1453,8 @@
     </row>
     <row r="30" spans="1:38" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
-      <c r="B30" s="25"/>
-      <c r="C30" s="26"/>
+      <c r="B30" s="26"/>
+      <c r="C30" s="27"/>
       <c r="D30" s="10"/>
       <c r="E30" s="11"/>
       <c r="F30" s="12"/>
@@ -1449,8 +1467,8 @@
     </row>
     <row r="31" spans="1:38" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
-      <c r="B31" s="25"/>
-      <c r="C31" s="26"/>
+      <c r="B31" s="26"/>
+      <c r="C31" s="27"/>
       <c r="D31" s="10"/>
       <c r="E31" s="11"/>
       <c r="F31" s="12"/>
@@ -1463,8 +1481,8 @@
     </row>
     <row r="32" spans="1:38" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
-      <c r="B32" s="25"/>
-      <c r="C32" s="26"/>
+      <c r="B32" s="26"/>
+      <c r="C32" s="27"/>
       <c r="D32" s="10"/>
       <c r="E32" s="11"/>
       <c r="F32" s="12"/>
@@ -9506,6 +9524,31 @@
     </row>
   </sheetData>
   <mergeCells count="32">
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B25:C25"/>
     <mergeCell ref="B31:C31"/>
     <mergeCell ref="B32:C32"/>
     <mergeCell ref="B26:C26"/>
@@ -9513,31 +9556,6 @@
     <mergeCell ref="B28:C28"/>
     <mergeCell ref="B29:C29"/>
     <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="B1:G1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -9548,8 +9566,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:E10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -9559,10 +9577,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="29"/>
+      <c r="B1" s="21"/>
       <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
@@ -9577,10 +9595,10 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A2" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2" s="27"/>
+      <c r="A2" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="19"/>
       <c r="C2" s="10">
         <v>5</v>
       </c>
@@ -9591,15 +9609,15 @@
         <v>5</v>
       </c>
       <c r="F2" s="13">
-        <f>C2+D2+E2</f>
+        <f t="shared" ref="F2:F10" si="0">C2+D2+E2</f>
         <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="28"/>
+      <c r="B3" s="20"/>
       <c r="C3" s="10">
         <v>3</v>
       </c>
@@ -9610,15 +9628,15 @@
         <v>4</v>
       </c>
       <c r="F3" s="13">
-        <f>C3+D3+E3</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A4" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="B4" s="28"/>
+      <c r="A4" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="20"/>
       <c r="C4" s="10">
         <v>4</v>
       </c>
@@ -9629,15 +9647,15 @@
         <v>4</v>
       </c>
       <c r="F4" s="13">
-        <f>C4+D4+E4</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A5" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="B5" s="27"/>
+      <c r="A5" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="19"/>
       <c r="C5" s="10">
         <v>5</v>
       </c>
@@ -9648,15 +9666,15 @@
         <v>1</v>
       </c>
       <c r="F5" s="13">
-        <f>C5+D5+E5</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A6" s="28" t="s">
+      <c r="A6" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="B6" s="28"/>
+      <c r="B6" s="20"/>
       <c r="C6" s="10">
         <v>4</v>
       </c>
@@ -9667,15 +9685,15 @@
         <v>3</v>
       </c>
       <c r="F6" s="13">
-        <f>C6+D6+E6</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A7" s="28" t="s">
-        <v>30</v>
-      </c>
-      <c r="B7" s="28"/>
+      <c r="A7" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" s="20"/>
       <c r="C7" s="10">
         <v>2</v>
       </c>
@@ -9686,15 +9704,15 @@
         <v>3</v>
       </c>
       <c r="F7" s="13">
-        <f>C7+D7+E7</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A8" s="27" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" s="27"/>
+      <c r="A8" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="19"/>
       <c r="C8" s="10">
         <v>3</v>
       </c>
@@ -9705,15 +9723,15 @@
         <v>1</v>
       </c>
       <c r="F8" s="13">
-        <f>C8+D8+E8</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A9" s="27" t="s">
+      <c r="A9" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="27"/>
+      <c r="B9" s="19"/>
       <c r="C9" s="10">
         <v>2</v>
       </c>
@@ -9724,15 +9742,15 @@
         <v>2</v>
       </c>
       <c r="F9" s="13">
-        <f>C9+D9+E9</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="28" t="s">
-        <v>33</v>
-      </c>
-      <c r="B10" s="28"/>
+      <c r="A10" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" s="20"/>
       <c r="C10" s="10">
         <v>2</v>
       </c>
@@ -9743,7 +9761,7 @@
         <v>2</v>
       </c>
       <c r="F10" s="13">
-        <f>C10+D10+E10</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>

</xml_diff>